<commit_message>
Update to a few things related to analysis
</commit_message>
<xml_diff>
--- a/data-raw/dap.xlsx
+++ b/data-raw/dap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillaume.noblet\Documents\GitHub\impactR\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC3C86E-2117-4B6D-AE71-C5D49FFF0194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8DD23C-1AC7-407D-A1AB-C8696A73C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dap" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>id_analysis</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Aléatoire</t>
   </si>
   <si>
-    <t>h_3_type_latrine_latrine_prive,i_enum_id</t>
-  </si>
-  <si>
     <t>Ratio</t>
   </si>
   <si>
@@ -142,13 +139,52 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>none_label</t>
+  </si>
+  <si>
+    <t>Genre de l'enquêté/e non chef/fe de ménage</t>
+  </si>
+  <si>
+    <t>c_n_chef_menage_genre</t>
+  </si>
+  <si>
+    <t>Parmi les ménages dont le répondant/e n'est pas le ou la cheffe de ménage</t>
+  </si>
+  <si>
+    <t>prop_simple</t>
+  </si>
+  <si>
+    <t>analysis_5</t>
+  </si>
+  <si>
+    <t>analysis_6</t>
+  </si>
+  <si>
+    <t>analysis_7</t>
+  </si>
+  <si>
+    <t>prop_simple_overall</t>
+  </si>
+  <si>
+    <t>Répondant/e chef/fe de ménage</t>
+  </si>
+  <si>
+    <t>h_3_type_latrine_latrine_prive,r_besoin_assistance_eha</t>
+  </si>
+  <si>
+    <t>Ménages rapportant des latrines privées parmi les ménages rapportant un besoin d'assistance en EHA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,28 +211,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Leelawadee"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Leelawadee"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF333333"/>
-        <bgColor rgb="FF333300"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -228,41 +268,674 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Leelawadee"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Leelawadee UI"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -273,6 +946,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB0FE79-6F28-4AF7-8AD2-58DA48D2E436}" name="Table2" displayName="Table2" ref="A1:O1048576" totalsRowShown="0" headerRowDxfId="17" dataDxfId="0" tableBorderDxfId="16">
+  <autoFilter ref="A1:O1048576" xr:uid="{CBB0FE79-6F28-4AF7-8AD2-58DA48D2E436}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{CF6E96C9-3084-48A6-9680-39BB1A97B2FE}" name="id_analysis" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{2569CB63-528B-419F-89CD-0A34A6B31DFB}" name="rq" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{3398810B-225F-4694-9B07-D67C54AF5EF1}" name="sub_rq" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1FEC1B8F-D0D9-4B9E-9EE6-8A51740B6C13}" name="indicator" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{10F18DDD-CF09-4C2E-A395-447C5BA33480}" name="recall" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{D8BB71D5-9A6A-427B-B0DE-6FB6D2DE1A75}" name="question_name" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{280CEE7F-7B69-49E8-B6F2-720AF55DB76B}" name="subset" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{CCFDD668-AA72-408D-8A4F-3A1DDAC42FB2}" name="analysis_name" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{EF61CD21-B37D-4E62-B153-4CB446A6E1E0}" name="analysis" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{C1916389-89ED-4F08-99CF-C0A6802AA57C}" name="none_label" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{45572B42-9C1B-4D30-AF7A-D1B07118EC15}" name="group_name" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{F1FDFFF3-CE0B-49DC-9EF8-B6CDB05AB8DE}" name="group" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{872A0A60-FB7E-4FB6-9BD3-9B895E4D0ACD}" name="level" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{0380BC98-905E-485A-95FB-48D90E2C84CD}" name="na_rm" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{967AF1C2-A0DA-4B44-9A32-A9520015A74A}" name="vartype" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,273 +1269,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AML13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19" style="1" customWidth="1"/>
-    <col min="10" max="1023" width="11.5703125" style="1"/>
-    <col min="1024" max="1024" width="11.5703125" style="2"/>
+    <col min="1" max="1" width="10.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="14" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="15" customWidth="1"/>
+    <col min="16" max="1026" width="11.5703125" style="4"/>
+    <col min="1027" max="16384" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15 1026:1026" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AMJ1" s="6"/>
+      <c r="AML1" s="1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="11"/>
+      <c r="K2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11">
         <v>0.9</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="N2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ2" s="8"/>
     </row>
-    <row r="3" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="7">
+      <c r="M3" s="11">
         <v>0.9</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ3" s="8"/>
     </row>
-    <row r="4" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="B5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L5" s="11"/>
+      <c r="M5" s="11">
         <v>0.9</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="N5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="O5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ4" s="8"/>
     </row>
-    <row r="5" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="7">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11">
         <v>0.9</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="N6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="O6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ5" s="8"/>
     </row>
-    <row r="6" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:15 1026:1026" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="7">
+      <c r="L7" s="11"/>
+      <c r="M7" s="11">
         <v>0.9</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="N7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="O7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ6" s="8"/>
     </row>
-    <row r="7" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ7" s="8"/>
+    <row r="8" spans="1:15 1026:1026" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ8" s="8"/>
+    <row r="9" spans="1:15 1026:1026" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="12"/>
     </row>
-    <row r="9" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ9" s="8"/>
+    <row r="10" spans="1:15 1026:1026" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="12"/>
     </row>
-    <row r="10" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ10" s="8"/>
+    <row r="11" spans="1:15 1026:1026" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="12"/>
     </row>
-    <row r="11" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ11" s="8"/>
+    <row r="12" spans="1:15 1026:1026" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="12"/>
     </row>
-    <row r="12" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ12" s="8"/>
-    </row>
-    <row r="13" spans="1:1024" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AMJ13" s="8"/>
+    <row r="13" spans="1:15 1026:1026" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>